<commit_message>
update form hoa don
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying\Java_KiemThu\BaiTapLon\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9DBF82-E909-4389-B59D-7A17A62F259D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case" sheetId="2" r:id="rId2"/>
     <sheet name="Test Report" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1448,7 +1454,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
@@ -1456,7 +1462,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2094,6 +2100,60 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2132,60 +2192,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2211,7 +2217,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Functional Test Case v1.0" xfId="1"/>
+    <cellStyle name="Normal_Functional Test Case v1.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2496,23 +2502,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="15.59765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.19921875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" customHeight="1">
+    <row r="1" spans="1:17" ht="16.95" customHeight="1">
       <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2539,7 @@
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
     </row>
-    <row r="2" spans="1:17" ht="11.5" customHeight="1">
+    <row r="2" spans="1:17" ht="11.55" customHeight="1">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -2552,7 +2558,7 @@
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" ht="14.5" customHeight="1">
+    <row r="3" spans="1:17" ht="14.55" customHeight="1">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2571,7 +2577,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="14.5" customHeight="1" outlineLevel="1">
+    <row r="4" spans="1:17" ht="14.55" customHeight="1" outlineLevel="1">
       <c r="A4" s="31" t="s">
         <v>31</v>
       </c>
@@ -2658,7 +2664,7 @@
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
     </row>
-    <row r="9" spans="1:17" ht="14.5" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="9" spans="1:17" ht="14.4" hidden="1" outlineLevel="1" thickBot="1">
       <c r="B9" s="32" t="s">
         <v>162</v>
       </c>
@@ -2923,7 +2929,7 @@
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
     </row>
-    <row r="21" spans="1:15" ht="14.5" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="21" spans="1:15" ht="14.4" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A21" s="19"/>
       <c r="B21" s="30">
         <v>12</v>
@@ -3028,67 +3034,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="18.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="43.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="56.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.453125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="60.90625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="23.08984375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="18.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="56.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.59765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="60.8984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.09765625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.69921875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="40.5" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="93"/>
-    </row>
-    <row r="2" spans="1:17" ht="14.5" customHeight="1" outlineLevel="1">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="77"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.55" customHeight="1" outlineLevel="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="93"/>
-    </row>
-    <row r="3" spans="1:17" ht="14.5" customHeight="1" outlineLevel="1">
+      <c r="H2" s="77"/>
+    </row>
+    <row r="3" spans="1:17" ht="14.55" customHeight="1" outlineLevel="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="93"/>
-    </row>
-    <row r="4" spans="1:17" ht="16" outlineLevel="1">
+      <c r="H3" s="77"/>
+    </row>
+    <row r="4" spans="1:17" ht="16.8" outlineLevel="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3103,12 +3109,12 @@
         <f xml:space="preserve"> COUNTIF(F:F, "Pending")</f>
         <v>16</v>
       </c>
-      <c r="E4" s="100"/>
+      <c r="E4" s="84"/>
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
-      <c r="H4" s="93"/>
-    </row>
-    <row r="5" spans="1:17" ht="16" outlineLevel="1">
+      <c r="H4" s="77"/>
+    </row>
+    <row r="5" spans="1:17" ht="16.8" outlineLevel="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3123,12 +3129,12 @@
         <f xml:space="preserve"> COUNTA(A9:A64)-12</f>
         <v>44</v>
       </c>
-      <c r="E5" s="100"/>
+      <c r="E5" s="84"/>
       <c r="F5" s="67"/>
       <c r="G5" s="67"/>
-      <c r="H5" s="93"/>
-    </row>
-    <row r="6" spans="1:17" s="93" customFormat="1"/>
+      <c r="H5" s="77"/>
+    </row>
+    <row r="6" spans="1:17" s="77" customFormat="1"/>
     <row r="7" spans="1:17" s="5" customFormat="1" ht="15">
       <c r="A7" s="4" t="s">
         <v>6</v>
@@ -3165,14 +3171,14 @@
       <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:17" ht="15">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
@@ -3184,15 +3190,15 @@
       <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="1:17" ht="19.5" customHeight="1">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="79" t="s">
         <v>227</v>
       </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
       <c r="H9" s="46" t="s">
         <v>224</v>
       </c>
@@ -3206,7 +3212,7 @@
       <c r="P9" s="45"/>
       <c r="Q9" s="45"/>
     </row>
-    <row r="10" spans="1:17" ht="80" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="10" spans="1:17" ht="79.95" customHeight="1" outlineLevel="1">
       <c r="A10" s="6" t="s">
         <v>87</v>
       </c>
@@ -3224,9 +3230,9 @@
         <v>14</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="74"/>
-    </row>
-    <row r="11" spans="1:17" ht="53.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H10" s="92"/>
+    </row>
+    <row r="11" spans="1:17" ht="53.55" customHeight="1" outlineLevel="1">
       <c r="A11" s="6" t="s">
         <v>88</v>
       </c>
@@ -3246,9 +3252,9 @@
       <c r="G11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="75"/>
-    </row>
-    <row r="12" spans="1:17" ht="51" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H11" s="93"/>
+    </row>
+    <row r="12" spans="1:17" ht="51" customHeight="1" outlineLevel="1">
       <c r="A12" s="6" t="s">
         <v>89</v>
       </c>
@@ -3266,9 +3272,9 @@
         <v>14</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="75"/>
-    </row>
-    <row r="13" spans="1:17" ht="65" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H12" s="93"/>
+    </row>
+    <row r="13" spans="1:17" ht="64.95" customHeight="1" outlineLevel="1">
       <c r="A13" s="6" t="s">
         <v>90</v>
       </c>
@@ -3288,9 +3294,9 @@
       <c r="G13" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="H13" s="75"/>
-    </row>
-    <row r="14" spans="1:17" ht="50.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H13" s="93"/>
+    </row>
+    <row r="14" spans="1:17" ht="50.55" customHeight="1" outlineLevel="1">
       <c r="A14" s="6" t="s">
         <v>91</v>
       </c>
@@ -3310,9 +3316,9 @@
       <c r="G14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="75"/>
-    </row>
-    <row r="15" spans="1:17" ht="50" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H14" s="93"/>
+    </row>
+    <row r="15" spans="1:17" ht="49.95" customHeight="1" outlineLevel="1">
       <c r="A15" s="6" t="s">
         <v>92</v>
       </c>
@@ -3330,9 +3336,9 @@
         <v>14</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="75"/>
-    </row>
-    <row r="16" spans="1:17" ht="37" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H15" s="93"/>
+    </row>
+    <row r="16" spans="1:17" ht="37.049999999999997" customHeight="1" outlineLevel="1">
       <c r="A16" s="6" t="s">
         <v>93</v>
       </c>
@@ -3350,9 +3356,9 @@
         <v>14</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="75"/>
-    </row>
-    <row r="17" spans="1:8" ht="34" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H16" s="93"/>
+    </row>
+    <row r="17" spans="1:8" ht="34.049999999999997" customHeight="1" outlineLevel="1">
       <c r="A17" s="6" t="s">
         <v>94</v>
       </c>
@@ -3370,23 +3376,23 @@
         <v>14</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="76"/>
-    </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" ht="18.5" customHeight="1" collapsed="1">
-      <c r="A18" s="86" t="s">
+      <c r="H17" s="94"/>
+    </row>
+    <row r="18" spans="1:8" s="10" customFormat="1" ht="18.45" customHeight="1">
+      <c r="A18" s="72" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="46" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="67" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="19" spans="1:8" ht="67.05" customHeight="1" outlineLevel="1">
       <c r="A19" s="6" t="s">
         <v>95</v>
       </c>
@@ -3408,9 +3414,9 @@
       <c r="G19" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="H19" s="77"/>
-    </row>
-    <row r="20" spans="1:8" ht="67" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H19" s="95"/>
+    </row>
+    <row r="20" spans="1:8" ht="67.05" customHeight="1" outlineLevel="1">
       <c r="A20" s="6" t="s">
         <v>96</v>
       </c>
@@ -3432,9 +3438,9 @@
       <c r="G20" s="51" t="s">
         <v>246</v>
       </c>
-      <c r="H20" s="78"/>
-    </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="89" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H20" s="96"/>
+    </row>
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="88.95" customHeight="1" outlineLevel="1">
       <c r="A21" s="6" t="s">
         <v>97</v>
       </c>
@@ -3456,9 +3462,9 @@
       <c r="G21" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="78"/>
-    </row>
-    <row r="22" spans="1:8" ht="164" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H21" s="96"/>
+    </row>
+    <row r="22" spans="1:8" ht="163.95" customHeight="1" outlineLevel="1">
       <c r="A22" s="6" t="s">
         <v>98</v>
       </c>
@@ -3480,9 +3486,9 @@
       <c r="G22" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="78"/>
-    </row>
-    <row r="23" spans="1:8" ht="58" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H22" s="96"/>
+    </row>
+    <row r="23" spans="1:8" ht="58.05" customHeight="1" outlineLevel="1">
       <c r="A23" s="6" t="s">
         <v>99</v>
       </c>
@@ -3502,9 +3508,9 @@
         <v>3</v>
       </c>
       <c r="G23" s="9"/>
-      <c r="H23" s="78"/>
-    </row>
-    <row r="24" spans="1:8" ht="37" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H23" s="96"/>
+    </row>
+    <row r="24" spans="1:8" ht="37.049999999999997" customHeight="1" outlineLevel="1">
       <c r="A24" s="6" t="s">
         <v>100</v>
       </c>
@@ -3524,23 +3530,23 @@
         <v>3</v>
       </c>
       <c r="G24" s="9"/>
-      <c r="H24" s="79"/>
-    </row>
-    <row r="25" spans="1:8" s="10" customFormat="1" ht="20" customHeight="1" collapsed="1">
-      <c r="A25" s="86" t="s">
+      <c r="H24" s="97"/>
+    </row>
+    <row r="25" spans="1:8" s="10" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A25" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
       <c r="H25" s="46" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="39" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="26" spans="1:8" ht="39" customHeight="1" outlineLevel="1">
       <c r="A26" s="34" t="s">
         <v>101</v>
       </c>
@@ -3562,16 +3568,16 @@
       </c>
       <c r="H26" s="47"/>
     </row>
-    <row r="27" spans="1:8" s="10" customFormat="1" ht="19.5" customHeight="1" collapsed="1">
-      <c r="A27" s="86" t="s">
+    <row r="27" spans="1:8" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A27" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
       <c r="H27" s="46" t="s">
         <v>224</v>
       </c>
@@ -3598,7 +3604,7 @@
       <c r="G28" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="H28" s="80"/>
+      <c r="H28" s="98"/>
     </row>
     <row r="29" spans="1:8" ht="66" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A29" s="34" t="s">
@@ -3622,9 +3628,9 @@
       <c r="G29" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="H29" s="81"/>
-    </row>
-    <row r="30" spans="1:8" ht="39.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H29" s="99"/>
+    </row>
+    <row r="30" spans="1:8" ht="39.450000000000003" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A30" s="34" t="s">
         <v>104</v>
       </c>
@@ -3646,9 +3652,9 @@
       <c r="G30" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="81"/>
-    </row>
-    <row r="31" spans="1:8" ht="54.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H30" s="99"/>
+    </row>
+    <row r="31" spans="1:8" ht="54.45" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A31" s="37" t="s">
         <v>105</v>
       </c>
@@ -3670,18 +3676,18 @@
       <c r="G31" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="H31" s="82"/>
-    </row>
-    <row r="32" spans="1:8" s="13" customFormat="1" ht="19" customHeight="1" collapsed="1">
-      <c r="A32" s="86" t="s">
+      <c r="H31" s="100"/>
+    </row>
+    <row r="32" spans="1:8" s="13" customFormat="1" ht="19.05" customHeight="1" collapsed="1">
+      <c r="A32" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
       <c r="H32" s="46" t="s">
         <v>226</v>
       </c>
@@ -3703,12 +3709,12 @@
       <c r="F33" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="94" t="s">
+      <c r="G33" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="H33" s="80"/>
-    </row>
-    <row r="34" spans="1:8" ht="58" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H33" s="98"/>
+    </row>
+    <row r="34" spans="1:8" ht="58.05" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A34" s="6" t="s">
         <v>107</v>
       </c>
@@ -3725,10 +3731,10 @@
       <c r="F34" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="94"/>
-      <c r="H34" s="81"/>
-    </row>
-    <row r="35" spans="1:8" ht="55" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="G34" s="78"/>
+      <c r="H34" s="99"/>
+    </row>
+    <row r="35" spans="1:8" ht="55.05" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A35" s="6" t="s">
         <v>108</v>
       </c>
@@ -3745,24 +3751,24 @@
       <c r="F35" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="94"/>
-      <c r="H35" s="82"/>
-    </row>
-    <row r="36" spans="1:8" s="13" customFormat="1" ht="20.5" customHeight="1" collapsed="1">
-      <c r="A36" s="86" t="s">
+      <c r="G35" s="78"/>
+      <c r="H35" s="100"/>
+    </row>
+    <row r="36" spans="1:8" s="13" customFormat="1" ht="20.55" customHeight="1" collapsed="1">
+      <c r="A36" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
       <c r="H36" s="46" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="195" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="37" spans="1:8" ht="195" customHeight="1" outlineLevel="1">
       <c r="A37" s="16" t="s">
         <v>109</v>
       </c>
@@ -3784,9 +3790,9 @@
       <c r="G37" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="80"/>
-    </row>
-    <row r="38" spans="1:8" ht="40.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H37" s="98"/>
+    </row>
+    <row r="38" spans="1:8" ht="40.5" customHeight="1" outlineLevel="1">
       <c r="A38" s="16" t="s">
         <v>110</v>
       </c>
@@ -3808,23 +3814,23 @@
       <c r="G38" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="H38" s="82"/>
-    </row>
-    <row r="39" spans="1:8" ht="21" customHeight="1" collapsed="1">
-      <c r="A39" s="83" t="s">
+      <c r="H38" s="100"/>
+    </row>
+    <row r="39" spans="1:8" ht="21" customHeight="1">
+      <c r="A39" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="B39" s="84"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="84"/>
-      <c r="F39" s="84"/>
-      <c r="G39" s="85"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="87"/>
       <c r="H39" s="46" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="107" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="40" spans="1:8" ht="106.95" customHeight="1" outlineLevel="1">
       <c r="A40" s="16" t="s">
         <v>111</v>
       </c>
@@ -3846,9 +3852,9 @@
       <c r="G40" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="H40" s="80"/>
-    </row>
-    <row r="41" spans="1:8" ht="48" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H40" s="98"/>
+    </row>
+    <row r="41" spans="1:8" ht="48" customHeight="1" outlineLevel="1">
       <c r="A41" s="16" t="s">
         <v>112</v>
       </c>
@@ -3868,23 +3874,23 @@
         <v>3</v>
       </c>
       <c r="G41" s="36"/>
-      <c r="H41" s="82"/>
-    </row>
-    <row r="42" spans="1:8" ht="19" customHeight="1" collapsed="1">
-      <c r="A42" s="83" t="s">
+      <c r="H41" s="100"/>
+    </row>
+    <row r="42" spans="1:8" ht="19.05" customHeight="1">
+      <c r="A42" s="85" t="s">
         <v>203</v>
       </c>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
-      <c r="F42" s="84"/>
-      <c r="G42" s="85"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="87"/>
       <c r="H42" s="46" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="47.5" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="43" spans="1:8" ht="47.55" customHeight="1" outlineLevel="1">
       <c r="A43" s="34" t="s">
         <v>114</v>
       </c>
@@ -3906,9 +3912,9 @@
       <c r="G43" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H43" s="80"/>
-    </row>
-    <row r="44" spans="1:8" ht="68" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H43" s="98"/>
+    </row>
+    <row r="44" spans="1:8" ht="67.95" customHeight="1" outlineLevel="1">
       <c r="A44" s="16" t="s">
         <v>119</v>
       </c>
@@ -3930,23 +3936,23 @@
       <c r="G44" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="H44" s="82"/>
-    </row>
-    <row r="45" spans="1:8" ht="16.5" customHeight="1" collapsed="1">
-      <c r="A45" s="83" t="s">
+      <c r="H44" s="100"/>
+    </row>
+    <row r="45" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A45" s="85" t="s">
         <v>204</v>
       </c>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="85"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="87"/>
       <c r="H45" s="46" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="45" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:8" ht="45" outlineLevel="1">
       <c r="A46" s="16" t="s">
         <v>136</v>
       </c>
@@ -3970,21 +3976,21 @@
       </c>
       <c r="H46" s="48"/>
     </row>
-    <row r="47" spans="1:8" ht="16.5" customHeight="1" collapsed="1">
-      <c r="A47" s="89" t="s">
+    <row r="47" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A47" s="73" t="s">
         <v>230</v>
       </c>
-      <c r="B47" s="90"/>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="91"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="75"/>
       <c r="H47" s="46" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="66" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="48" spans="1:8" ht="66" customHeight="1" outlineLevel="1">
       <c r="A48" s="6" t="s">
         <v>137</v>
       </c>
@@ -4001,12 +4007,12 @@
       <c r="F48" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="92" t="s">
+      <c r="G48" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="H48" s="80"/>
-    </row>
-    <row r="49" spans="1:8" ht="35" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H48" s="98"/>
+    </row>
+    <row r="49" spans="1:8" ht="34.950000000000003" customHeight="1" outlineLevel="1">
       <c r="A49" s="6" t="s">
         <v>138</v>
       </c>
@@ -4023,10 +4029,10 @@
       <c r="F49" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G49" s="92"/>
-      <c r="H49" s="81"/>
-    </row>
-    <row r="50" spans="1:8" ht="36.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="G49" s="76"/>
+      <c r="H49" s="99"/>
+    </row>
+    <row r="50" spans="1:8" ht="36.450000000000003" customHeight="1" outlineLevel="1">
       <c r="A50" s="6" t="s">
         <v>139</v>
       </c>
@@ -4043,24 +4049,24 @@
       <c r="F50" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="92"/>
-      <c r="H50" s="82"/>
-    </row>
-    <row r="51" spans="1:8" ht="19" customHeight="1" collapsed="1">
-      <c r="A51" s="83" t="s">
+      <c r="G50" s="76"/>
+      <c r="H50" s="100"/>
+    </row>
+    <row r="51" spans="1:8" ht="19.05" customHeight="1">
+      <c r="A51" s="85" t="s">
         <v>205</v>
       </c>
-      <c r="B51" s="84"/>
-      <c r="C51" s="84"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="85"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="87"/>
       <c r="H51" s="46" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="58" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="52" spans="1:8" ht="58.05" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A52" s="16" t="s">
         <v>140</v>
       </c>
@@ -4082,21 +4088,21 @@
       </c>
       <c r="H52" s="49"/>
     </row>
-    <row r="53" spans="1:8" s="10" customFormat="1" ht="20.5" customHeight="1" collapsed="1">
-      <c r="A53" s="86" t="s">
+    <row r="53" spans="1:8" s="10" customFormat="1" ht="20.55" customHeight="1" collapsed="1">
+      <c r="A53" s="72" t="s">
         <v>231</v>
       </c>
-      <c r="B53" s="86"/>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="72"/>
+      <c r="F53" s="72"/>
+      <c r="G53" s="72"/>
       <c r="H53" s="46" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="64" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="54" spans="1:8" ht="64.05" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A54" s="34" t="s">
         <v>141</v>
       </c>
@@ -4118,7 +4124,7 @@
       <c r="G54" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="H54" s="70"/>
+      <c r="H54" s="88"/>
     </row>
     <row r="55" spans="1:8" ht="55.5" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A55" s="34" t="s">
@@ -4140,7 +4146,7 @@
         <v>3</v>
       </c>
       <c r="G55" s="43"/>
-      <c r="H55" s="71"/>
+      <c r="H55" s="89"/>
     </row>
     <row r="56" spans="1:8" ht="52.5" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A56" s="34" t="s">
@@ -4164,7 +4170,7 @@
       <c r="G56" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="H56" s="71"/>
+      <c r="H56" s="89"/>
     </row>
     <row r="57" spans="1:8" ht="55.5" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A57" s="34" t="s">
@@ -4188,9 +4194,9 @@
       <c r="G57" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="H57" s="71"/>
-    </row>
-    <row r="58" spans="1:8" ht="36.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H57" s="89"/>
+    </row>
+    <row r="58" spans="1:8" ht="36.450000000000003" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A58" s="34" t="s">
         <v>209</v>
       </c>
@@ -4210,9 +4216,9 @@
         <v>3</v>
       </c>
       <c r="G58" s="44"/>
-      <c r="H58" s="71"/>
-    </row>
-    <row r="59" spans="1:8" ht="80" hidden="1" customHeight="1" outlineLevel="1" collapsed="1">
+      <c r="H58" s="89"/>
+    </row>
+    <row r="59" spans="1:8" ht="79.95" hidden="1" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="A59" s="34" t="s">
         <v>210</v>
       </c>
@@ -4234,9 +4240,9 @@
       <c r="G59" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="H59" s="71"/>
-    </row>
-    <row r="60" spans="1:8" ht="56.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H59" s="89"/>
+    </row>
+    <row r="60" spans="1:8" ht="56.55" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A60" s="34" t="s">
         <v>211</v>
       </c>
@@ -4258,7 +4264,7 @@
       <c r="G60" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="H60" s="71"/>
+      <c r="H60" s="89"/>
     </row>
     <row r="61" spans="1:8" ht="52.5" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A61" s="34" t="s">
@@ -4282,9 +4288,9 @@
       <c r="G61" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="H61" s="71"/>
-    </row>
-    <row r="62" spans="1:8" ht="77.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H61" s="89"/>
+    </row>
+    <row r="62" spans="1:8" ht="77.55" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A62" s="34" t="s">
         <v>217</v>
       </c>
@@ -4306,9 +4312,9 @@
       <c r="G62" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="H62" s="71"/>
-    </row>
-    <row r="63" spans="1:8" ht="57.5" hidden="1" customHeight="1" outlineLevel="1">
+      <c r="H62" s="89"/>
+    </row>
+    <row r="63" spans="1:8" ht="57.45" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A63" s="34" t="s">
         <v>219</v>
       </c>
@@ -4328,7 +4334,7 @@
         <v>3</v>
       </c>
       <c r="G63" s="14"/>
-      <c r="H63" s="71"/>
+      <c r="H63" s="89"/>
     </row>
     <row r="64" spans="1:8" ht="64.5" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A64" s="34" t="s">
@@ -4352,11 +4358,25 @@
       <c r="G64" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="H64" s="72"/>
+      <c r="H64" s="90"/>
     </row>
     <row r="65" collapsed="1"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H54:H64"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="H19:H24"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="H48:H50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="A36:G36"/>
@@ -4373,20 +4393,6 @@
     <mergeCell ref="C2:D3"/>
     <mergeCell ref="E4:G5"/>
     <mergeCell ref="A45:G45"/>
-    <mergeCell ref="H54:H64"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H19:H24"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="H48:H50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4394,23 +4400,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="6.90625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.8984375" style="3" customWidth="1"/>
     <col min="2" max="2" width="26" style="3" customWidth="1"/>
-    <col min="3" max="5" width="8.7265625" style="3"/>
-    <col min="6" max="6" width="22.7265625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="3"/>
+    <col min="3" max="5" width="8.69921875" style="3"/>
+    <col min="6" max="6" width="22.69921875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.69921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.5">
+    <row r="1" spans="1:6" ht="24.6">
       <c r="A1" s="101" t="s">
         <v>35</v>
       </c>

</xml_diff>